<commit_message>
Auto commit - 2024-08-07
</commit_message>
<xml_diff>
--- a/2024/2024_06_07_CB_loans/2_Money_Base_eng.xlsx
+++ b/2024/2024_06_07_CB_loans/2_Money_Base_eng.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\_INTERNET-databank\1. Monetary Sector\1-Monetary indicators-25\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\FOR ALL\_INTERNET-databank\1. Monetary Sector\1-Monetary indicators-25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2285DEB8-C540-4A0D-A8DA-24CC02EC27E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2AAF36-1292-47F3-9C31-14B11BE9BE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2903,7 +2903,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="112">
   <si>
     <t xml:space="preserve">(end of period, million drams) </t>
   </si>
@@ -4227,6 +4227,21 @@
         <family val="1"/>
       </rPr>
       <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Jun-24 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Times Armenian"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
     </r>
   </si>
 </sst>
@@ -6033,7 +6048,7 @@
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="150" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="150" applyFont="1" applyFill="1"/>
@@ -6093,6 +6108,7 @@
     <xf numFmtId="3" fontId="48" fillId="0" borderId="11" xfId="150" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="0" xfId="150" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="596">
     <cellStyle name=" Verticals" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -7085,13 +7101,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IX31"/>
+  <dimension ref="A1:JC31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="IN5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="JB22" sqref="JB22"/>
+      <selection pane="bottomRight" activeCell="IU27" sqref="IU27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7186,24 +7202,24 @@
     <col min="206" max="217" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="218" max="219" width="10.85546875" style="2" customWidth="1"/>
     <col min="220" max="220" width="11.85546875" style="2" customWidth="1"/>
-    <col min="221" max="258" width="10.85546875" style="2" customWidth="1"/>
-    <col min="259" max="16384" width="9.140625" style="2"/>
+    <col min="221" max="259" width="10.85546875" style="2" customWidth="1"/>
+    <col min="260" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:258" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:263" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:258" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:263" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:258" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:263" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:258" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:263" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="18"/>
       <c r="B4" s="17">
         <v>37622</v>
@@ -7976,8 +7992,11 @@
       <c r="IX4" s="17">
         <v>45440</v>
       </c>
+      <c r="IY4" s="17" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="5" spans="1:258" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:263" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -8236,8 +8255,9 @@
       <c r="IV5" s="5"/>
       <c r="IW5" s="5"/>
       <c r="IX5" s="5"/>
+      <c r="IY5" s="5"/>
     </row>
-    <row r="6" spans="1:258" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:263" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
@@ -9012,8 +9032,12 @@
       <c r="IX6" s="25">
         <v>926820.54863712401</v>
       </c>
+      <c r="IY6" s="25">
+        <v>984774.87543887529</v>
+      </c>
+      <c r="JC6" s="27"/>
     </row>
-    <row r="7" spans="1:258" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:263" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -9272,8 +9296,10 @@
       <c r="IV7" s="26"/>
       <c r="IW7" s="26"/>
       <c r="IX7" s="26"/>
+      <c r="IY7" s="26"/>
+      <c r="JC7" s="27"/>
     </row>
-    <row r="8" spans="1:258" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:263" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>24</v>
       </c>
@@ -10048,8 +10074,12 @@
       <c r="IX8" s="26">
         <v>714078.87732437626</v>
       </c>
+      <c r="IY8" s="26">
+        <v>862170.15462282463</v>
+      </c>
+      <c r="JC8" s="27"/>
     </row>
-    <row r="9" spans="1:258" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>25</v>
       </c>
@@ -10824,8 +10854,12 @@
       <c r="IX9" s="24">
         <v>-437181.55686550005</v>
       </c>
+      <c r="IY9" s="24">
+        <v>-486536.34381640004</v>
+      </c>
+      <c r="JC9" s="27"/>
     </row>
-    <row r="10" spans="1:258" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>26</v>
       </c>
@@ -11600,8 +11634,12 @@
       <c r="IX10" s="24">
         <v>684017.04693659989</v>
       </c>
+      <c r="IY10" s="24">
+        <v>884164.04184159997</v>
+      </c>
+      <c r="JC10" s="27"/>
     </row>
-    <row r="11" spans="1:258" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>40</v>
       </c>
@@ -12376,8 +12414,12 @@
       <c r="IX11" s="24">
         <v>385170.51719799999</v>
       </c>
+      <c r="IY11" s="24">
+        <v>581524.16789300006</v>
+      </c>
+      <c r="JC11" s="27"/>
     </row>
-    <row r="12" spans="1:258" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>27</v>
       </c>
@@ -13132,8 +13174,12 @@
       <c r="IX12" s="24">
         <v>0</v>
       </c>
+      <c r="IY12" s="24">
+        <v>0</v>
+      </c>
+      <c r="JC12" s="27"/>
     </row>
-    <row r="13" spans="1:258" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>28</v>
       </c>
@@ -13906,8 +13952,12 @@
       <c r="IX13" s="24">
         <v>0</v>
       </c>
+      <c r="IY13" s="24">
+        <v>0</v>
+      </c>
+      <c r="JC13" s="27"/>
     </row>
-    <row r="14" spans="1:258" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>29</v>
       </c>
@@ -14680,8 +14730,12 @@
       <c r="IX14" s="24">
         <v>0</v>
       </c>
+      <c r="IY14" s="24">
+        <v>0</v>
+      </c>
+      <c r="JC14" s="27"/>
     </row>
-    <row r="15" spans="1:258" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>30</v>
       </c>
@@ -15448,8 +15502,12 @@
       <c r="IX15" s="24">
         <v>0</v>
       </c>
+      <c r="IY15" s="24">
+        <v>0</v>
+      </c>
+      <c r="JC15" s="27"/>
     </row>
-    <row r="16" spans="1:258" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>31</v>
       </c>
@@ -16164,8 +16222,12 @@
       <c r="IX16" s="24">
         <v>0</v>
       </c>
+      <c r="IY16" s="24">
+        <v>0</v>
+      </c>
+      <c r="JC16" s="27"/>
     </row>
-    <row r="17" spans="1:258" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>32</v>
       </c>
@@ -16940,8 +17002,12 @@
       <c r="IX17" s="24">
         <v>467243.38725327642</v>
       </c>
+      <c r="IY17" s="24">
+        <v>464542.4565976247</v>
+      </c>
+      <c r="JC17" s="27"/>
     </row>
-    <row r="18" spans="1:258" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:263" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -17202,8 +17268,10 @@
       <c r="IV18" s="26"/>
       <c r="IW18" s="26"/>
       <c r="IX18" s="26"/>
+      <c r="IY18" s="26"/>
+      <c r="JC18" s="27"/>
     </row>
-    <row r="19" spans="1:258" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:263" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>33</v>
       </c>
@@ -17978,8 +18046,12 @@
       <c r="IX19" s="26">
         <v>1640899.4259615003</v>
       </c>
+      <c r="IY19" s="26">
+        <v>1846945.0300616999</v>
+      </c>
+      <c r="JC19" s="27"/>
     </row>
-    <row r="20" spans="1:258" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>34</v>
       </c>
@@ -18754,8 +18826,12 @@
       <c r="IX20" s="24">
         <v>855915.59543370001</v>
       </c>
+      <c r="IY20" s="24">
+        <v>885265.76098079991</v>
+      </c>
+      <c r="JC20" s="27"/>
     </row>
-    <row r="21" spans="1:258" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>64</v>
       </c>
@@ -19530,8 +19606,12 @@
       <c r="IX21" s="24">
         <v>326487.09865230002</v>
       </c>
+      <c r="IY21" s="24">
+        <v>488146.60069170006</v>
+      </c>
+      <c r="JC21" s="27"/>
     </row>
-    <row r="22" spans="1:258" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>63</v>
       </c>
@@ -20248,8 +20328,12 @@
       <c r="IX22" s="24">
         <v>440339.05141649995</v>
       </c>
+      <c r="IY22" s="24">
+        <v>454921.29308029998</v>
+      </c>
+      <c r="JC22" s="27"/>
     </row>
-    <row r="23" spans="1:258" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>35</v>
       </c>
@@ -21024,8 +21108,12 @@
       <c r="IX23" s="24">
         <v>18157.680459000287</v>
       </c>
+      <c r="IY23" s="24">
+        <v>18611.375308899966</v>
+      </c>
+      <c r="JC23" s="27"/>
     </row>
-    <row r="24" spans="1:258" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>65</v>
       </c>
@@ -21800,8 +21888,12 @@
       <c r="IX24" s="24">
         <v>15208.810871400001</v>
       </c>
+      <c r="IY24" s="24">
+        <v>15775.263899500002</v>
+      </c>
+      <c r="JC24" s="27"/>
     </row>
-    <row r="25" spans="1:258" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>66</v>
       </c>
@@ -22576,23 +22668,30 @@
       <c r="IX25" s="24">
         <v>2948.8695875999997</v>
       </c>
+      <c r="IY25" s="24">
+        <v>2836.1114094000004</v>
+      </c>
+      <c r="JC25" s="27"/>
     </row>
-    <row r="27" spans="1:258" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:263" x14ac:dyDescent="0.2">
+      <c r="JC26" s="27"/>
+    </row>
+    <row r="27" spans="1:263" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:258" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:263" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:258" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:263" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:258" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:263" x14ac:dyDescent="0.2">
       <c r="A31" s="19"/>
     </row>
   </sheetData>
@@ -34423,13 +34522,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{601FB487-440F-49E8-BDFB-3878E7D26C54}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42FAE247-2A64-413F-A39B-C7B6954573D5}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F75CBA9-82C0-4FC1-B860-494826550A3B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5705369F-39C2-4C0E-A6AC-9FD99393EBE4}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0293ACEE-6E2F-4769-B0FE-9251E3613E0C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{086E3B1B-6527-4930-8E9E-2BCF3728E8F9}"/>
 </file>
</xml_diff>

<commit_message>
Auto commit - 2024-09-04
</commit_message>
<xml_diff>
--- a/2024/2024_06_07_CB_loans/2_Money_Base_eng.xlsx
+++ b/2024/2024_06_07_CB_loans/2_Money_Base_eng.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\FOR ALL\_INTERNET-databank\1. Monetary Sector\1-Monetary indicators-25\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\_INTERNET-databank\1. Monetary Sector\1-Monetary indicators-25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2AAF36-1292-47F3-9C31-14B11BE9BE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90762B70-4069-4505-BBD9-8D02749AB455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7107,7 +7107,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="IN5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="IU27" sqref="IU27"/>
+      <selection pane="bottomRight" activeCell="JC18" sqref="JC18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7202,8 +7202,8 @@
     <col min="206" max="217" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="218" max="219" width="10.85546875" style="2" customWidth="1"/>
     <col min="220" max="220" width="11.85546875" style="2" customWidth="1"/>
-    <col min="221" max="259" width="10.85546875" style="2" customWidth="1"/>
-    <col min="260" max="16384" width="9.140625" style="2"/>
+    <col min="221" max="260" width="10.85546875" style="2" customWidth="1"/>
+    <col min="261" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:263" ht="15" x14ac:dyDescent="0.2">
@@ -7994,6 +7994,9 @@
       </c>
       <c r="IY4" s="17" t="s">
         <v>111</v>
+      </c>
+      <c r="IZ4" s="17">
+        <v>45501</v>
       </c>
     </row>
     <row r="5" spans="1:263" x14ac:dyDescent="0.2">
@@ -8256,6 +8259,7 @@
       <c r="IW5" s="5"/>
       <c r="IX5" s="5"/>
       <c r="IY5" s="5"/>
+      <c r="IZ5" s="5"/>
     </row>
     <row r="6" spans="1:263" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -9034,6 +9038,9 @@
       </c>
       <c r="IY6" s="25">
         <v>984774.87543887529</v>
+      </c>
+      <c r="IZ6" s="25">
+        <v>1011279.8879208271</v>
       </c>
       <c r="JC6" s="27"/>
     </row>
@@ -9297,6 +9304,7 @@
       <c r="IW7" s="26"/>
       <c r="IX7" s="26"/>
       <c r="IY7" s="26"/>
+      <c r="IZ7" s="26"/>
       <c r="JC7" s="27"/>
     </row>
     <row r="8" spans="1:263" ht="14.25" x14ac:dyDescent="0.25">
@@ -10077,6 +10085,9 @@
       <c r="IY8" s="26">
         <v>862170.15462282463</v>
       </c>
+      <c r="IZ8" s="26">
+        <v>680660.75837427308</v>
+      </c>
       <c r="JC8" s="27"/>
     </row>
     <row r="9" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -10857,6 +10868,9 @@
       <c r="IY9" s="24">
         <v>-486536.34381640004</v>
       </c>
+      <c r="IZ9" s="24">
+        <v>-489204.6266134</v>
+      </c>
       <c r="JC9" s="27"/>
     </row>
     <row r="10" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -11637,6 +11651,9 @@
       <c r="IY10" s="24">
         <v>884164.04184159997</v>
       </c>
+      <c r="IZ10" s="24">
+        <v>714162.81608050002</v>
+      </c>
       <c r="JC10" s="27"/>
     </row>
     <row r="11" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -12416,6 +12433,9 @@
       </c>
       <c r="IY11" s="24">
         <v>581524.16789300006</v>
+      </c>
+      <c r="IZ11" s="24">
+        <v>410000</v>
       </c>
       <c r="JC11" s="27"/>
     </row>
@@ -13177,6 +13197,9 @@
       <c r="IY12" s="24">
         <v>0</v>
       </c>
+      <c r="IZ12" s="24">
+        <v>0</v>
+      </c>
       <c r="JC12" s="27"/>
     </row>
     <row r="13" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -13955,6 +13978,9 @@
       <c r="IY13" s="24">
         <v>0</v>
       </c>
+      <c r="IZ13" s="24">
+        <v>0</v>
+      </c>
       <c r="JC13" s="27"/>
     </row>
     <row r="14" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -14733,6 +14759,9 @@
       <c r="IY14" s="24">
         <v>0</v>
       </c>
+      <c r="IZ14" s="24">
+        <v>0</v>
+      </c>
       <c r="JC14" s="27"/>
     </row>
     <row r="15" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -15503,6 +15532,9 @@
         <v>0</v>
       </c>
       <c r="IY15" s="24">
+        <v>0</v>
+      </c>
+      <c r="IZ15" s="24">
         <v>0</v>
       </c>
       <c r="JC15" s="27"/>
@@ -16225,6 +16257,9 @@
       <c r="IY16" s="24">
         <v>0</v>
       </c>
+      <c r="IZ16" s="24">
+        <v>0</v>
+      </c>
       <c r="JC16" s="27"/>
     </row>
     <row r="17" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -17004,6 +17039,9 @@
       </c>
       <c r="IY17" s="24">
         <v>464542.4565976247</v>
+      </c>
+      <c r="IZ17" s="24">
+        <v>455702.568907173</v>
       </c>
       <c r="JC17" s="27"/>
     </row>
@@ -17269,6 +17307,7 @@
       <c r="IW18" s="26"/>
       <c r="IX18" s="26"/>
       <c r="IY18" s="26"/>
+      <c r="IZ18" s="26"/>
       <c r="JC18" s="27"/>
     </row>
     <row r="19" spans="1:263" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
@@ -18049,6 +18088,9 @@
       <c r="IY19" s="26">
         <v>1846945.0300616999</v>
       </c>
+      <c r="IZ19" s="26">
+        <v>1691940.6462951002</v>
+      </c>
       <c r="JC19" s="27"/>
     </row>
     <row r="20" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -18829,6 +18871,9 @@
       <c r="IY20" s="24">
         <v>885265.76098079991</v>
       </c>
+      <c r="IZ20" s="24">
+        <v>915032.53519300011</v>
+      </c>
       <c r="JC20" s="27"/>
     </row>
     <row r="21" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -19608,6 +19653,9 @@
       </c>
       <c r="IY21" s="24">
         <v>488146.60069170006</v>
+      </c>
+      <c r="IZ21" s="24">
+        <v>293960.56550990004</v>
       </c>
       <c r="JC21" s="27"/>
     </row>
@@ -20331,6 +20379,9 @@
       <c r="IY22" s="24">
         <v>454921.29308029998</v>
       </c>
+      <c r="IZ22" s="24">
+        <v>462789.00924079999</v>
+      </c>
       <c r="JC22" s="27"/>
     </row>
     <row r="23" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -21111,6 +21162,9 @@
       <c r="IY23" s="24">
         <v>18611.375308899966</v>
       </c>
+      <c r="IZ23" s="24">
+        <v>20158.536351400078</v>
+      </c>
       <c r="JC23" s="27"/>
     </row>
     <row r="24" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -21891,6 +21945,9 @@
       <c r="IY24" s="24">
         <v>15775.263899500002</v>
       </c>
+      <c r="IZ24" s="24">
+        <v>16865.764892799998</v>
+      </c>
       <c r="JC24" s="27"/>
     </row>
     <row r="25" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -22670,6 +22727,9 @@
       </c>
       <c r="IY25" s="24">
         <v>2836.1114094000004</v>
+      </c>
+      <c r="IZ25" s="24">
+        <v>3292.7714586000002</v>
       </c>
       <c r="JC25" s="27"/>
     </row>
@@ -34522,13 +34582,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42FAE247-2A64-413F-A39B-C7B6954573D5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E8E8E53-E372-4695-896E-688B0442C7C8}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5705369F-39C2-4C0E-A6AC-9FD99393EBE4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C42839D-95EB-4134-9C0C-C6F536D9D8D6}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{086E3B1B-6527-4930-8E9E-2BCF3728E8F9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87D86773-13C7-4F5A-9705-DB8D552690D2}"/>
 </file>
</xml_diff>

<commit_message>
Auto commit - 2024-09-27
</commit_message>
<xml_diff>
--- a/2024/2024_06_07_CB_loans/2_Money_Base_eng.xlsx
+++ b/2024/2024_06_07_CB_loans/2_Money_Base_eng.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\_INTERNET-databank\1. Monetary Sector\1-Monetary indicators-25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90762B70-4069-4505-BBD9-8D02749AB455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B510006-88F9-482C-9860-61044AC07998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4241,7 +4241,7 @@
         <rFont val="Times Armenian"/>
         <family val="1"/>
       </rPr>
-      <t>3</t>
+      <t>2</t>
     </r>
   </si>
 </sst>
@@ -7107,7 +7107,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="IN5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="JC18" sqref="JC18"/>
+      <selection pane="bottomRight" activeCell="IS30" sqref="IS30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7202,8 +7202,8 @@
     <col min="206" max="217" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="218" max="219" width="10.85546875" style="2" customWidth="1"/>
     <col min="220" max="220" width="11.85546875" style="2" customWidth="1"/>
-    <col min="221" max="260" width="10.85546875" style="2" customWidth="1"/>
-    <col min="261" max="16384" width="9.140625" style="2"/>
+    <col min="221" max="261" width="10.85546875" style="2" customWidth="1"/>
+    <col min="262" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:263" ht="15" x14ac:dyDescent="0.2">
@@ -7997,6 +7997,9 @@
       </c>
       <c r="IZ4" s="17">
         <v>45501</v>
+      </c>
+      <c r="JA4" s="17">
+        <v>45532</v>
       </c>
     </row>
     <row r="5" spans="1:263" x14ac:dyDescent="0.2">
@@ -8260,6 +8263,7 @@
       <c r="IX5" s="5"/>
       <c r="IY5" s="5"/>
       <c r="IZ5" s="5"/>
+      <c r="JA5" s="5"/>
     </row>
     <row r="6" spans="1:263" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -9037,10 +9041,13 @@
         <v>926820.54863712401</v>
       </c>
       <c r="IY6" s="25">
-        <v>984774.87543887529</v>
+        <v>988499.13655198901</v>
       </c>
       <c r="IZ6" s="25">
         <v>1011279.8879208271</v>
+      </c>
+      <c r="JA6" s="25">
+        <v>1081889.7866975579</v>
       </c>
       <c r="JC6" s="27"/>
     </row>
@@ -9305,6 +9312,7 @@
       <c r="IX7" s="26"/>
       <c r="IY7" s="26"/>
       <c r="IZ7" s="26"/>
+      <c r="JA7" s="26"/>
       <c r="JC7" s="27"/>
     </row>
     <row r="8" spans="1:263" ht="14.25" x14ac:dyDescent="0.25">
@@ -10083,10 +10091,13 @@
         <v>714078.87732437626</v>
       </c>
       <c r="IY8" s="26">
-        <v>862170.15462282463</v>
+        <v>858445.89350971091</v>
       </c>
       <c r="IZ8" s="26">
         <v>680660.75837427308</v>
+      </c>
+      <c r="JA8" s="26">
+        <v>702668.27182374219</v>
       </c>
       <c r="JC8" s="27"/>
     </row>
@@ -10871,6 +10882,9 @@
       <c r="IZ9" s="24">
         <v>-489204.6266134</v>
       </c>
+      <c r="JA9" s="24">
+        <v>-486586.92172869999</v>
+      </c>
       <c r="JC9" s="27"/>
     </row>
     <row r="10" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -11649,10 +11663,13 @@
         <v>684017.04693659989</v>
       </c>
       <c r="IY10" s="24">
-        <v>884164.04184159997</v>
+        <v>885048.99702929996</v>
       </c>
       <c r="IZ10" s="24">
         <v>714162.81608050002</v>
+      </c>
+      <c r="JA10" s="24">
+        <v>741348.17518090014</v>
       </c>
       <c r="JC10" s="27"/>
     </row>
@@ -12436,6 +12453,9 @@
       </c>
       <c r="IZ11" s="24">
         <v>410000</v>
+      </c>
+      <c r="JA11" s="24">
+        <v>430278.74866699998</v>
       </c>
       <c r="JC11" s="27"/>
     </row>
@@ -13200,6 +13220,9 @@
       <c r="IZ12" s="24">
         <v>0</v>
       </c>
+      <c r="JA12" s="24">
+        <v>0</v>
+      </c>
       <c r="JC12" s="27"/>
     </row>
     <row r="13" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -13981,6 +14004,9 @@
       <c r="IZ13" s="24">
         <v>0</v>
       </c>
+      <c r="JA13" s="24">
+        <v>0</v>
+      </c>
       <c r="JC13" s="27"/>
     </row>
     <row r="14" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -14762,6 +14788,9 @@
       <c r="IZ14" s="24">
         <v>0</v>
       </c>
+      <c r="JA14" s="24">
+        <v>0</v>
+      </c>
       <c r="JC14" s="27"/>
     </row>
     <row r="15" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -15535,6 +15564,9 @@
         <v>0</v>
       </c>
       <c r="IZ15" s="24">
+        <v>0</v>
+      </c>
+      <c r="JA15" s="24">
         <v>0</v>
       </c>
       <c r="JC15" s="27"/>
@@ -16260,6 +16292,9 @@
       <c r="IZ16" s="24">
         <v>0</v>
       </c>
+      <c r="JA16" s="24">
+        <v>0</v>
+      </c>
       <c r="JC16" s="27"/>
     </row>
     <row r="17" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -17038,10 +17073,13 @@
         <v>467243.38725327642</v>
       </c>
       <c r="IY17" s="24">
-        <v>464542.4565976247</v>
+        <v>459933.24029681098</v>
       </c>
       <c r="IZ17" s="24">
         <v>455702.568907173</v>
+      </c>
+      <c r="JA17" s="24">
+        <v>447907.01837154198</v>
       </c>
       <c r="JC17" s="27"/>
     </row>
@@ -17308,6 +17346,7 @@
       <c r="IX18" s="26"/>
       <c r="IY18" s="26"/>
       <c r="IZ18" s="26"/>
+      <c r="JA18" s="26"/>
       <c r="JC18" s="27"/>
     </row>
     <row r="19" spans="1:263" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
@@ -18091,6 +18130,9 @@
       <c r="IZ19" s="26">
         <v>1691940.6462951002</v>
       </c>
+      <c r="JA19" s="26">
+        <v>1784558.0585213001</v>
+      </c>
       <c r="JC19" s="27"/>
     </row>
     <row r="20" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -18874,6 +18916,9 @@
       <c r="IZ20" s="24">
         <v>915032.53519300011</v>
       </c>
+      <c r="JA20" s="24">
+        <v>930076.05141179997</v>
+      </c>
       <c r="JC20" s="27"/>
     </row>
     <row r="21" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -19656,6 +19701,9 @@
       </c>
       <c r="IZ21" s="24">
         <v>293960.56550990004</v>
+      </c>
+      <c r="JA21" s="24">
+        <v>336468.20764670003</v>
       </c>
       <c r="JC21" s="27"/>
     </row>
@@ -20382,6 +20430,9 @@
       <c r="IZ22" s="24">
         <v>462789.00924079999</v>
       </c>
+      <c r="JA22" s="24">
+        <v>496521.53092709999</v>
+      </c>
       <c r="JC22" s="27"/>
     </row>
     <row r="23" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -21165,6 +21216,9 @@
       <c r="IZ23" s="24">
         <v>20158.536351400078</v>
       </c>
+      <c r="JA23" s="24">
+        <v>21492.268535700103</v>
+      </c>
       <c r="JC23" s="27"/>
     </row>
     <row r="24" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -21948,6 +22002,9 @@
       <c r="IZ24" s="24">
         <v>16865.764892799998</v>
       </c>
+      <c r="JA24" s="24">
+        <v>16951.532343300001</v>
+      </c>
       <c r="JC24" s="27"/>
     </row>
     <row r="25" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
@@ -22730,6 +22787,9 @@
       </c>
       <c r="IZ25" s="24">
         <v>3292.7714586000002</v>
+      </c>
+      <c r="JA25" s="24">
+        <v>4540.7361923999997</v>
       </c>
       <c r="JC25" s="27"/>
     </row>
@@ -34582,13 +34642,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E8E8E53-E372-4695-896E-688B0442C7C8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78F39449-D883-4712-B86C-E5C3A2AD9218}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C42839D-95EB-4134-9C0C-C6F536D9D8D6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFF9546E-1D1D-42F9-BFD0-12C99BBA695B}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87D86773-13C7-4F5A-9705-DB8D552690D2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8DF18B9-4695-4FBC-8119-51132D69C5EA}"/>
 </file>
</xml_diff>

<commit_message>
Auto commit - 2025-01-29
</commit_message>
<xml_diff>
--- a/2024/2024_06_07_CB_loans/2_Money_Base_eng.xlsx
+++ b/2024/2024_06_07_CB_loans/2_Money_Base_eng.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\_INTERNET-databank\1. Monetary Sector\1-Monetary indicators-25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC88ADD-61B7-44CA-9BC0-36183966C46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA1751C-AC7D-4D2C-B5BB-F7FB35595B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2903,7 +2903,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="116">
   <si>
     <t xml:space="preserve">(end of period, million drams) </t>
   </si>
@@ -4263,6 +4263,21 @@
         <family val="1"/>
       </rPr>
       <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dec-24 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Times Armenian"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
     </r>
   </si>
 </sst>
@@ -6742,7 +6757,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -6761,7 +6776,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -6780,7 +6795,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Ü»ñ·ñ³íí³Í"/>
@@ -6801,9 +6816,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6841,9 +6856,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6876,26 +6891,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6928,26 +6926,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7121,13 +7102,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:JC33"/>
+  <dimension ref="A1:JE33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="IS5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="JI24" sqref="JI24"/>
+      <selection pane="bottomRight" activeCell="JH21" sqref="JH21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7222,24 +7203,24 @@
     <col min="206" max="217" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="218" max="219" width="10.85546875" style="2" customWidth="1"/>
     <col min="220" max="220" width="11.85546875" style="2" customWidth="1"/>
-    <col min="221" max="263" width="10.85546875" style="2" customWidth="1"/>
-    <col min="264" max="16384" width="9.140625" style="2"/>
+    <col min="221" max="265" width="10.85546875" style="2" customWidth="1"/>
+    <col min="266" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:263" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:265" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:263" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:265" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:263" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:265" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:263" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:265" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="18"/>
       <c r="B4" s="17">
         <v>37622</v>
@@ -8027,8 +8008,14 @@
       <c r="JC4" s="17">
         <v>45593</v>
       </c>
+      <c r="JD4" s="17">
+        <v>45624</v>
+      </c>
+      <c r="JE4" s="17" t="s">
+        <v>115</v>
+      </c>
     </row>
-    <row r="5" spans="1:263" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:265" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -8292,8 +8279,10 @@
       <c r="JA5" s="5"/>
       <c r="JB5" s="5"/>
       <c r="JC5" s="5"/>
+      <c r="JD5" s="5"/>
+      <c r="JE5" s="5"/>
     </row>
-    <row r="6" spans="1:263" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:265" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
@@ -9083,8 +9072,14 @@
       <c r="JC6" s="25">
         <v>1074200.0022660706</v>
       </c>
+      <c r="JD6" s="25">
+        <v>1083955.8238674009</v>
+      </c>
+      <c r="JE6" s="25">
+        <v>1139532.031125471</v>
+      </c>
     </row>
-    <row r="7" spans="1:263" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:265" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -9348,8 +9343,10 @@
       <c r="JA7" s="26"/>
       <c r="JB7" s="26"/>
       <c r="JC7" s="26"/>
+      <c r="JD7" s="26"/>
+      <c r="JE7" s="26"/>
     </row>
-    <row r="8" spans="1:263" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:265" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>24</v>
       </c>
@@ -10110,28 +10107,28 @@
         <v>727922.80212156218</v>
       </c>
       <c r="IT8" s="26">
-        <v>572855.07030861243</v>
+        <v>572855.10023661237</v>
       </c>
       <c r="IU8" s="26">
-        <v>619370.28832124709</v>
+        <v>619370.31824924704</v>
       </c>
       <c r="IV8" s="26">
-        <v>765844.46968078311</v>
+        <v>765844.49960878305</v>
       </c>
       <c r="IW8" s="26">
-        <v>783156.19883118756</v>
+        <v>783156.22875918774</v>
       </c>
       <c r="IX8" s="26">
-        <v>714078.87732437626</v>
+        <v>714079.39463237626</v>
       </c>
       <c r="IY8" s="26">
-        <v>858445.89350971091</v>
+        <v>858446.93857371085</v>
       </c>
       <c r="IZ8" s="26">
-        <v>680660.75837427308</v>
+        <v>680662.61279467307</v>
       </c>
       <c r="JA8" s="26">
-        <v>702668.27182374219</v>
+        <v>702813.01564704208</v>
       </c>
       <c r="JB8" s="26">
         <v>847488.4706827749</v>
@@ -10139,8 +10136,14 @@
       <c r="JC8" s="26">
         <v>672192.01087752893</v>
       </c>
+      <c r="JD8" s="26">
+        <v>593957.60201579914</v>
+      </c>
+      <c r="JE8" s="26">
+        <v>960372.5621636291</v>
+      </c>
     </row>
-    <row r="9" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>25</v>
       </c>
@@ -10930,8 +10933,14 @@
       <c r="JC9" s="24">
         <v>-439828.62110599998</v>
       </c>
+      <c r="JD9" s="24">
+        <v>-467697.09767589998</v>
+      </c>
+      <c r="JE9" s="24">
+        <v>-419370.82706649997</v>
+      </c>
     </row>
-    <row r="10" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>26</v>
       </c>
@@ -11721,8 +11730,14 @@
       <c r="JC10" s="24">
         <v>677416.91447760002</v>
       </c>
+      <c r="JD10" s="24">
+        <v>637638.86670239992</v>
+      </c>
+      <c r="JE10" s="24">
+        <v>961309.24881999998</v>
+      </c>
     </row>
-    <row r="11" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>40</v>
       </c>
@@ -12512,8 +12527,14 @@
       <c r="JC11" s="24">
         <v>375076.02791599999</v>
       </c>
+      <c r="JD11" s="24">
+        <v>330201.69154000003</v>
+      </c>
+      <c r="JE11" s="24">
+        <v>651281.90015499992</v>
+      </c>
     </row>
-    <row r="12" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>27</v>
       </c>
@@ -13253,38 +13274,22 @@
       <c r="IS12" s="24">
         <v>0</v>
       </c>
-      <c r="IT12" s="24">
-        <v>0</v>
-      </c>
-      <c r="IU12" s="24">
-        <v>0</v>
-      </c>
-      <c r="IV12" s="24">
-        <v>0</v>
-      </c>
-      <c r="IW12" s="24">
-        <v>0</v>
-      </c>
-      <c r="IX12" s="24">
-        <v>0</v>
-      </c>
-      <c r="IY12" s="24">
-        <v>0</v>
-      </c>
-      <c r="IZ12" s="24">
-        <v>0</v>
-      </c>
-      <c r="JA12" s="24">
-        <v>0</v>
-      </c>
-      <c r="JB12" s="24">
-        <v>0</v>
-      </c>
-      <c r="JC12" s="24">
+      <c r="IT12" s="24"/>
+      <c r="IU12" s="24"/>
+      <c r="IV12" s="24"/>
+      <c r="IW12" s="24"/>
+      <c r="IX12" s="24"/>
+      <c r="IY12" s="24"/>
+      <c r="IZ12" s="24"/>
+      <c r="JA12" s="24"/>
+      <c r="JB12" s="24"/>
+      <c r="JC12" s="24"/>
+      <c r="JD12" s="24"/>
+      <c r="JE12" s="24">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>28</v>
       </c>
@@ -14072,8 +14077,14 @@
       <c r="JC13" s="24">
         <v>0</v>
       </c>
+      <c r="JD13" s="24">
+        <v>0</v>
+      </c>
+      <c r="JE13" s="24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>29</v>
       </c>
@@ -14861,8 +14872,14 @@
       <c r="JC14" s="24">
         <v>0</v>
       </c>
+      <c r="JD14" s="24">
+        <v>0</v>
+      </c>
+      <c r="JE14" s="24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>30</v>
       </c>
@@ -15644,8 +15661,14 @@
       <c r="JC15" s="24">
         <v>0</v>
       </c>
+      <c r="JD15" s="24">
+        <v>0</v>
+      </c>
+      <c r="JE15" s="24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>31</v>
       </c>
@@ -16375,8 +16398,14 @@
       <c r="JC16" s="24">
         <v>0</v>
       </c>
+      <c r="JD16" s="24">
+        <v>0</v>
+      </c>
+      <c r="JE16" s="24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>32</v>
       </c>
@@ -17137,37 +17166,43 @@
         <v>452623.75134816219</v>
       </c>
       <c r="IT17" s="24">
-        <v>455736.11115331249</v>
+        <v>455736.14108131244</v>
       </c>
       <c r="IU17" s="24">
-        <v>454388.04765994719</v>
+        <v>454388.07758794737</v>
       </c>
       <c r="IV17" s="24">
-        <v>459829.67476498312</v>
+        <v>459829.70469298307</v>
       </c>
       <c r="IW17" s="24">
-        <v>468985.93967448769</v>
+        <v>468985.96960248786</v>
       </c>
       <c r="IX17" s="24">
-        <v>467243.38725327642</v>
+        <v>467243.90456127643</v>
       </c>
       <c r="IY17" s="24">
-        <v>459933.24029681098</v>
+        <v>459934.28536081093</v>
       </c>
       <c r="IZ17" s="24">
-        <v>455702.568907173</v>
+        <v>455704.42332757299</v>
       </c>
       <c r="JA17" s="24">
-        <v>447907.01837154198</v>
+        <v>448051.76219484187</v>
       </c>
       <c r="JB17" s="24">
-        <v>436008.89850369212</v>
+        <v>436008.89850387478</v>
       </c>
       <c r="JC17" s="24">
         <v>434603.71750592883</v>
       </c>
+      <c r="JD17" s="24">
+        <v>424015.8329892992</v>
+      </c>
+      <c r="JE17" s="24">
+        <v>418434.1404101291</v>
+      </c>
     </row>
-    <row r="18" spans="1:263" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:265" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -17433,8 +17468,10 @@
       <c r="JA18" s="26"/>
       <c r="JB18" s="26"/>
       <c r="JC18" s="26"/>
+      <c r="JD18" s="26"/>
+      <c r="JE18" s="26"/>
     </row>
-    <row r="19" spans="1:263" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:265" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>33</v>
       </c>
@@ -18195,28 +18232,28 @@
         <v>1845623.3761258002</v>
       </c>
       <c r="IT19" s="26">
-        <v>1679946.2623457001</v>
+        <v>1679946.2922737</v>
       </c>
       <c r="IU19" s="26">
-        <v>1649790.6211099999</v>
+        <v>1649790.6510379999</v>
       </c>
       <c r="IV19" s="26">
-        <v>1737133.6538599001</v>
+        <v>1737133.6837879</v>
       </c>
       <c r="IW19" s="26">
-        <v>1686351.3380156998</v>
+        <v>1686351.3679436999</v>
       </c>
       <c r="IX19" s="26">
-        <v>1640899.4259615003</v>
+        <v>1640899.9432695003</v>
       </c>
       <c r="IY19" s="26">
-        <v>1846945.0300616999</v>
+        <v>1846946.0751256999</v>
       </c>
       <c r="IZ19" s="26">
-        <v>1691940.6462951002</v>
+        <v>1691942.5007155002</v>
       </c>
       <c r="JA19" s="26">
-        <v>1784558.0585213001</v>
+        <v>1784702.8023446</v>
       </c>
       <c r="JB19" s="26">
         <v>1913867.5623837998</v>
@@ -18224,8 +18261,14 @@
       <c r="JC19" s="26">
         <v>1746392.0131435995</v>
       </c>
+      <c r="JD19" s="26">
+        <v>1677913.4258832</v>
+      </c>
+      <c r="JE19" s="26">
+        <v>2099904.5932891001</v>
+      </c>
     </row>
-    <row r="20" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>34</v>
       </c>
@@ -19015,8 +19058,14 @@
       <c r="JC20" s="24">
         <v>923087.6008306999</v>
       </c>
+      <c r="JD20" s="24">
+        <v>922478.20883469982</v>
+      </c>
+      <c r="JE20" s="24">
+        <v>986374.01862089988</v>
+      </c>
     </row>
-    <row r="21" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>64</v>
       </c>
@@ -19806,8 +19855,14 @@
       <c r="JC21" s="24">
         <v>342187.53954359994</v>
       </c>
+      <c r="JD21" s="24">
+        <v>277674.68888430001</v>
+      </c>
+      <c r="JE21" s="24">
+        <v>567463.57737630012</v>
+      </c>
     </row>
-    <row r="22" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>63</v>
       </c>
@@ -20539,8 +20594,14 @@
       <c r="JC22" s="24">
         <v>462118.49991959997</v>
       </c>
+      <c r="JD22" s="24">
+        <v>463927.57805729995</v>
+      </c>
+      <c r="JE22" s="24">
+        <v>518672.48830070003</v>
+      </c>
     </row>
-    <row r="23" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>112</v>
       </c>
@@ -20796,22 +20857,44 @@
       <c r="IQ23" s="24"/>
       <c r="IR23" s="24"/>
       <c r="IS23" s="24"/>
-      <c r="IT23" s="24"/>
-      <c r="IU23" s="24"/>
-      <c r="IV23" s="24"/>
-      <c r="IW23" s="24"/>
-      <c r="IX23" s="24"/>
-      <c r="IY23" s="24"/>
-      <c r="IZ23" s="24"/>
-      <c r="JA23" s="24"/>
+      <c r="IT23" s="24">
+        <v>2.9928E-2</v>
+      </c>
+      <c r="IU23" s="24">
+        <v>2.9928E-2</v>
+      </c>
+      <c r="IV23" s="24">
+        <v>2.9928E-2</v>
+      </c>
+      <c r="IW23" s="24">
+        <v>2.9928E-2</v>
+      </c>
+      <c r="IX23" s="24">
+        <v>0.12992799999999999</v>
+      </c>
+      <c r="IY23" s="24">
+        <v>0.22992799999999999</v>
+      </c>
+      <c r="IZ23" s="24">
+        <v>0.22192689999999998</v>
+      </c>
+      <c r="JA23" s="24">
+        <v>1.1020768000000001</v>
+      </c>
       <c r="JB23" s="24">
         <v>1.1020768000000001</v>
       </c>
       <c r="JC23" s="24">
         <v>1.1020768000000001</v>
       </c>
+      <c r="JD23" s="24">
+        <v>1.1688523</v>
+      </c>
+      <c r="JE23" s="24">
+        <v>0.82594699999999999</v>
+      </c>
     </row>
-    <row r="24" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>113</v>
       </c>
@@ -21067,22 +21150,44 @@
       <c r="IQ24" s="24"/>
       <c r="IR24" s="24"/>
       <c r="IS24" s="24"/>
-      <c r="IT24" s="24"/>
-      <c r="IU24" s="24"/>
-      <c r="IV24" s="24"/>
-      <c r="IW24" s="24"/>
-      <c r="IX24" s="24"/>
-      <c r="IY24" s="24"/>
-      <c r="IZ24" s="24"/>
-      <c r="JA24" s="24"/>
+      <c r="IT24" s="24">
+        <v>0</v>
+      </c>
+      <c r="IU24" s="24">
+        <v>0</v>
+      </c>
+      <c r="IV24" s="24">
+        <v>0</v>
+      </c>
+      <c r="IW24" s="24">
+        <v>0</v>
+      </c>
+      <c r="IX24" s="24">
+        <v>0.38738</v>
+      </c>
+      <c r="IY24" s="24">
+        <v>0.81513599999999997</v>
+      </c>
+      <c r="IZ24" s="24">
+        <v>1.6324935</v>
+      </c>
+      <c r="JA24" s="24">
+        <v>143.64174650000001</v>
+      </c>
       <c r="JB24" s="24">
         <v>143.92885219999999</v>
       </c>
       <c r="JC24" s="24">
         <v>142.936914</v>
       </c>
+      <c r="JD24" s="24">
+        <v>362.38806749999998</v>
+      </c>
+      <c r="JE24" s="24">
+        <v>1387.2403399</v>
+      </c>
     </row>
-    <row r="25" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>35</v>
       </c>
@@ -21843,28 +21948,28 @@
         <v>47966.948261700221</v>
       </c>
       <c r="IT25" s="24">
-        <v>19698.203578300017</v>
+        <v>19698.203578299963</v>
       </c>
       <c r="IU25" s="24">
-        <v>21770.781455199991</v>
+        <v>21770.781455199936</v>
       </c>
       <c r="IV25" s="24">
-        <v>18537.654393000237</v>
+        <v>18537.654393000183</v>
       </c>
       <c r="IW25" s="24">
-        <v>17200.077851099893</v>
+        <v>17200.077851100072</v>
       </c>
       <c r="IX25" s="24">
-        <v>18157.680459000287</v>
+        <v>18157.680459000298</v>
       </c>
       <c r="IY25" s="24">
-        <v>18611.375308899966</v>
+        <v>18611.375308899911</v>
       </c>
       <c r="IZ25" s="24">
-        <v>20158.536351400078</v>
+        <v>20158.536351400067</v>
       </c>
       <c r="JA25" s="24">
-        <v>21492.268535700103</v>
+        <v>21492.268535699983</v>
       </c>
       <c r="JB25" s="24">
         <v>18079.464525799791</v>
@@ -21872,8 +21977,14 @@
       <c r="JC25" s="24">
         <v>18854.333858899688</v>
       </c>
+      <c r="JD25" s="24">
+        <v>13469.393187100244</v>
+      </c>
+      <c r="JE25" s="24">
+        <v>26006.442704300069</v>
+      </c>
     </row>
-    <row r="26" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>65</v>
       </c>
@@ -22663,8 +22774,14 @@
       <c r="JC26" s="24">
         <v>14343.5603558</v>
       </c>
+      <c r="JD26" s="24">
+        <v>9905.134274500002</v>
+      </c>
+      <c r="JE26" s="24">
+        <v>23044.776054099999</v>
+      </c>
     </row>
-    <row r="27" spans="1:263" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:265" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>66</v>
       </c>
@@ -23454,18 +23571,24 @@
       <c r="JC27" s="24">
         <v>4510.7735031000002</v>
       </c>
+      <c r="JD27" s="24">
+        <v>3564.2589125999998</v>
+      </c>
+      <c r="JE27" s="24">
+        <v>2961.6666501999998</v>
+      </c>
     </row>
-    <row r="29" spans="1:263" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:265" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:263" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:265" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:263" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:265" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
         <v>67</v>
       </c>
@@ -35301,13 +35424,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C724DD08-6627-49CA-8CBE-FA0046F9F3D4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B07C6CB2-2154-41AE-B848-81D5BCD6C2CA}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EC0C-29DF-46D0-8A99-B051E3A3448E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6450EEE-1007-4057-B025-7515894F55E6}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE047907-016F-4024-A50C-6E52FEBADEF4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8141419-B4AD-4A5A-B96F-B96074136E42}"/>
 </file>
</xml_diff>